<commit_message>
Further Data Exploration and Visualisation
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D9391CD-A8CC-4E27-BBC4-6B0C57D58133}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E95146D1-2590-487C-BCD0-5B3012D718E1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{49574E81-5E76-4735-B155-75A7839EC357}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Develop and train supervised machine learning models using the training dataset. Experiment with different algorithms (logistic regression, decision trees, random forests, etc.) and hyperparameters. Evaluate the models using appropriate metrics (accuracy, precision, recall, F1-score) on the testing dataset.</t>
   </si>
   <si>
-    <t>Refine the machine learning models based on the insights gained from experiments and observations. Fine-tune the models' hyperparameters to optimize their performance. Validate the models' generalizability by testing them on unseen data.</t>
-  </si>
-  <si>
     <t>Conduct a comprehensive analysis of the experimental and observational results. Interpret the findings, discuss the significance of the variables, and evaluate the overall performance of the models.</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>Finalise the results and analysis section, including visualizations, tables, and statistical analyses. Write the discussion section, interpret the results, discuss their implications, and compare them to previous research. Start drafting the conclusion section, summarising the key findings, limitations, and recommendations for future research.</t>
+  </si>
+  <si>
+    <t>Focus on write-up. If needed, refine the machine learning models based on the insights gained from experiments and observations. Fine-tune the models' hyperparameters to optimize their performance. Validate the models' generalizability by testing them on unseen data.</t>
   </si>
 </sst>
 </file>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915AD513-53F8-40F4-A354-CA3E5A7D20AA}">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -524,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -556,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -564,7 +564,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interpret results of Chi Squared and Cramer's V tests to identify strength of relationships between categorical variables
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E95146D1-2590-487C-BCD0-5B3012D718E1}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEE14812-2315-4E59-B2BE-3A09DF7A6AC3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{49574E81-5E76-4735-B155-75A7839EC357}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49574E81-5E76-4735-B155-75A7839EC357}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915AD513-53F8-40F4-A354-CA3E5A7D20AA}">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ethics, IP  & NDA completed
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEE14812-2315-4E59-B2BE-3A09DF7A6AC3}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ABBC420-EB7B-49A7-9810-998C77947315}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49574E81-5E76-4735-B155-75A7839EC357}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{49574E81-5E76-4735-B155-75A7839EC357}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Timeline" sheetId="1" r:id="rId1"/>
+    <sheet name="Experimental Design" sheetId="2" r:id="rId2"/>
+    <sheet name="Experimental Plan" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Week</t>
   </si>
@@ -75,6 +77,135 @@
   </si>
   <si>
     <t>Focus on write-up. If needed, refine the machine learning models based on the insights gained from experiments and observations. Fine-tune the models' hyperparameters to optimize their performance. Validate the models' generalizability by testing them on unseen data.</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Data Preparation</t>
+  </si>
+  <si>
+    <t>Feature Selection</t>
+  </si>
+  <si>
+    <t>Sample Selection</t>
+  </si>
+  <si>
+    <t>Experimental Groups</t>
+  </si>
+  <si>
+    <t>Model Training</t>
+  </si>
+  <si>
+    <t>Model Evaluation</t>
+  </si>
+  <si>
+    <t>Validation and Generalisation</t>
+  </si>
+  <si>
+    <t>Conduct correlation analysis and calculate feature importances. Select top-n features.</t>
+  </si>
+  <si>
+    <t>Implement stratified random sampling to create a representative sample.</t>
+  </si>
+  <si>
+    <t>Divide the sample into multiple groups, each representing a different ML model.</t>
+  </si>
+  <si>
+    <t>Train each ML model using selected features and optimized hyperparameters.</t>
+  </si>
+  <si>
+    <t>Evaluate model performance on the training set using evaluation metrics.</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Collect and preprocess life assurance application dataset.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Expected Outcomes</t>
+  </si>
+  <si>
+    <t>Feature Impact Analysis</t>
+  </si>
+  <si>
+    <t>Identify features consistently contributing to model accuracy.</t>
+  </si>
+  <si>
+    <t>Model Comparison and Selection</t>
+  </si>
+  <si>
+    <t>Compare performance of different ML models in predicting application conversion.</t>
+  </si>
+  <si>
+    <t>Identify models with highest accuracy and assess hyperparameter contribution.</t>
+  </si>
+  <si>
+    <t>Test models on unseen test set to assess generalisability.</t>
+  </si>
+  <si>
+    <t>Analyse experimental results to identify features with significant impact on application conversion.</t>
+  </si>
+  <si>
+    <t>Test selected models on unseen test set.</t>
+  </si>
+  <si>
+    <t>Assess generalisability and validate model performance.</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Description and Notes</t>
+  </si>
+  <si>
+    <t>Model: Logistic Regression</t>
+  </si>
+  <si>
+    <t>Model: Random Forest</t>
+  </si>
+  <si>
+    <t>Model: Neural Network</t>
+  </si>
+  <si>
+    <t>Hyperparameter Tuning for Best Model</t>
+  </si>
+  <si>
+    <t>Model Evaluation with Test Data</t>
+  </si>
+  <si>
+    <t>Compare Model Performance and Select Best Model</t>
+  </si>
+  <si>
+    <t>Refine Best Model and Feature Importance Analysis</t>
+  </si>
+  <si>
+    <t>Interpretation of Model Results and Recommendations</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Model: Support Vector Machine</t>
+  </si>
+  <si>
+    <t>Validate Model on Unseen Data and Generalisation</t>
+  </si>
+  <si>
+    <t>Finalise Experimental Report and Documentation</t>
   </si>
 </sst>
 </file>
@@ -139,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -150,6 +281,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,110 +602,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915AD513-53F8-40F4-A354-CA3E5A7D20AA}">
-  <dimension ref="A2:B13"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -579,4 +713,278 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C607A7-8979-4A28-8F1E-9B2E3D8C8BAD}">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931071FD-A039-4A32-B87A-FB3F1F4290AD}">
+  <dimension ref="B2:D19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feature Importance - Random Forest Feature Importance Scoring
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3aa8172b9163bf4b/Documents/CCT/DataAnalytics/8.Capstone/Capstone Github Repository/MSc-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ABBC420-EB7B-49A7-9810-998C77947315}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{17ECA589-8393-4E8A-BEB3-681AA365B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FEB6C51-71E6-4D1A-8716-ADBF4001F5D4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{49574E81-5E76-4735-B155-75A7839EC357}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Week</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Finalise Experimental Report and Documentation</t>
+  </si>
+  <si>
+    <t>Model: Decision Tree</t>
   </si>
 </sst>
 </file>
@@ -814,10 +817,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931071FD-A039-4A32-B87A-FB3F1F4290AD}">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,7 +902,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -908,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -917,7 +920,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -926,7 +929,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -935,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -944,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -953,7 +956,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -962,7 +965,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -971,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -980,9 +983,18 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>